<commit_message>
update of recommender sample
</commit_message>
<xml_diff>
--- a/WebApi/Recommender Sample.xlsx
+++ b/WebApi/Recommender Sample.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chlu\git\Champion Selection Analyzer\WebApi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="18915" windowHeight="17955" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15240" windowHeight="6930" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Counters" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="109">
   <si>
     <t>Aatrox_Top</t>
   </si>
@@ -311,11 +316,44 @@
   <si>
     <t>Correct (not always announcements possible)</t>
   </si>
+  <si>
+    <t>pot. Announced</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>1. set own position -&gt; MID</t>
+  </si>
+  <si>
+    <t>2. counter: filter by other teams positions</t>
+  </si>
+  <si>
+    <t>3. counter: algorithm over enemy champs</t>
+  </si>
+  <si>
+    <t>4. synergy: filter by own teams positions</t>
+  </si>
+  <si>
+    <t>5. synergy: algorithm over team champs</t>
+  </si>
+  <si>
+    <t>Dictionary&lt;2DKey, &lt;2DKey, MatchUp&gt;&gt;</t>
+  </si>
+  <si>
+    <t>MatchUp:</t>
+  </si>
+  <si>
+    <t>CounterWinRate</t>
+  </si>
+  <si>
+    <t>SynergyWinRate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -592,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -655,14 +693,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -671,6 +703,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -681,14 +724,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -726,9 +772,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -763,7 +809,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -798,7 +844,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -975,7 +1021,7 @@
   <dimension ref="A1:BB51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,10 +1230,10 @@
       <c r="E2" s="37">
         <v>0</v>
       </c>
-      <c r="F2" s="37">
-        <v>0</v>
-      </c>
-      <c r="G2" s="30">
+      <c r="F2" s="62">
+        <v>0</v>
+      </c>
+      <c r="G2" s="33">
         <v>20</v>
       </c>
       <c r="H2" s="27">
@@ -1330,22 +1376,22 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31">
-        <v>20.04</v>
-      </c>
-      <c r="C3" s="28">
-        <v>69.12</v>
-      </c>
-      <c r="D3" s="5">
-        <v>14.15</v>
-      </c>
-      <c r="E3" s="25">
-        <v>95.09</v>
-      </c>
-      <c r="F3" s="22">
-        <v>49.73</v>
-      </c>
-      <c r="G3" s="31">
+      <c r="B3" s="41">
+        <v>0</v>
+      </c>
+      <c r="C3" s="39">
+        <v>0</v>
+      </c>
+      <c r="D3" s="39">
+        <v>0</v>
+      </c>
+      <c r="E3" s="39">
+        <v>0</v>
+      </c>
+      <c r="F3" s="40">
+        <v>0</v>
+      </c>
+      <c r="G3" s="34">
         <v>20.04</v>
       </c>
       <c r="H3" s="28">
@@ -1488,22 +1534,22 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31">
-        <v>20.079999999999998</v>
-      </c>
-      <c r="C4" s="28">
-        <v>69.13</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="25">
-        <v>91.13</v>
-      </c>
-      <c r="F4" s="22">
-        <v>46.22</v>
-      </c>
-      <c r="G4" s="31">
+      <c r="B4" s="41">
+        <v>0</v>
+      </c>
+      <c r="C4" s="39">
+        <v>0</v>
+      </c>
+      <c r="D4" s="39">
+        <v>0</v>
+      </c>
+      <c r="E4" s="39">
+        <v>0</v>
+      </c>
+      <c r="F4" s="40">
+        <v>0</v>
+      </c>
+      <c r="G4" s="34">
         <v>20.079999999999998</v>
       </c>
       <c r="H4" s="28">
@@ -1646,22 +1692,22 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="31">
-        <v>20.12</v>
-      </c>
-      <c r="C5" s="28">
-        <v>69.25</v>
-      </c>
-      <c r="D5" s="5">
-        <v>14.81</v>
-      </c>
-      <c r="E5" s="25">
-        <v>0</v>
-      </c>
-      <c r="F5" s="22">
-        <v>42.71</v>
-      </c>
-      <c r="G5" s="31">
+      <c r="B5" s="41">
+        <v>0</v>
+      </c>
+      <c r="C5" s="39">
+        <v>0</v>
+      </c>
+      <c r="D5" s="39">
+        <v>0</v>
+      </c>
+      <c r="E5" s="39">
+        <v>0</v>
+      </c>
+      <c r="F5" s="40">
+        <v>0</v>
+      </c>
+      <c r="G5" s="34">
         <v>20.12</v>
       </c>
       <c r="H5" s="28">
@@ -1804,22 +1850,22 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="32">
-        <v>20.16</v>
-      </c>
-      <c r="C6" s="29">
-        <v>69.37</v>
-      </c>
-      <c r="D6" s="6">
-        <v>15.14</v>
-      </c>
-      <c r="E6" s="26">
-        <v>83.21</v>
-      </c>
-      <c r="F6" s="23">
-        <v>39.200000000000003</v>
-      </c>
-      <c r="G6" s="32">
+      <c r="B6" s="63">
+        <v>0</v>
+      </c>
+      <c r="C6" s="64">
+        <v>0</v>
+      </c>
+      <c r="D6" s="64">
+        <v>0</v>
+      </c>
+      <c r="E6" s="64">
+        <v>0</v>
+      </c>
+      <c r="F6" s="65">
+        <v>0</v>
+      </c>
+      <c r="G6" s="35">
         <v>20.16</v>
       </c>
       <c r="H6" s="29">
@@ -1977,19 +2023,19 @@
       <c r="F7" s="22">
         <v>35.69</v>
       </c>
-      <c r="G7" s="41">
-        <v>0</v>
-      </c>
-      <c r="H7" s="39">
-        <v>0</v>
-      </c>
-      <c r="I7" s="39">
-        <v>0</v>
-      </c>
-      <c r="J7" s="39">
-        <v>0</v>
-      </c>
-      <c r="K7" s="40">
+      <c r="G7" s="36">
+        <v>0</v>
+      </c>
+      <c r="H7" s="37">
+        <v>0</v>
+      </c>
+      <c r="I7" s="37">
+        <v>0</v>
+      </c>
+      <c r="J7" s="37">
+        <v>0</v>
+      </c>
+      <c r="K7" s="62">
         <v>0</v>
       </c>
       <c r="L7" s="34">
@@ -2135,20 +2181,20 @@
       <c r="F8" s="22">
         <v>32.18</v>
       </c>
-      <c r="G8" s="31">
-        <v>20.239999999999998</v>
-      </c>
-      <c r="H8" s="28">
-        <v>15.8</v>
-      </c>
-      <c r="I8" s="5">
-        <v>15.8</v>
-      </c>
-      <c r="J8" s="25">
-        <v>75.290000000000006</v>
-      </c>
-      <c r="K8" s="19">
-        <v>32.18</v>
+      <c r="G8" s="41">
+        <v>0</v>
+      </c>
+      <c r="H8" s="39">
+        <v>0</v>
+      </c>
+      <c r="I8" s="39">
+        <v>0</v>
+      </c>
+      <c r="J8" s="39">
+        <v>0</v>
+      </c>
+      <c r="K8" s="40">
+        <v>0</v>
       </c>
       <c r="L8" s="34">
         <v>21.24</v>
@@ -2290,20 +2336,20 @@
       <c r="F9" s="22">
         <v>28.67</v>
       </c>
-      <c r="G9" s="31">
-        <v>20.28</v>
-      </c>
-      <c r="H9" s="28">
-        <v>16.13</v>
-      </c>
-      <c r="I9" s="5">
-        <v>16.13</v>
-      </c>
-      <c r="J9" s="25">
-        <v>71.33</v>
-      </c>
-      <c r="K9" s="19">
-        <v>28.67</v>
+      <c r="G9" s="41">
+        <v>0</v>
+      </c>
+      <c r="H9" s="39">
+        <v>0</v>
+      </c>
+      <c r="I9" s="39">
+        <v>0</v>
+      </c>
+      <c r="J9" s="39">
+        <v>0</v>
+      </c>
+      <c r="K9" s="40">
+        <v>0</v>
       </c>
       <c r="L9" s="34">
         <v>21.28</v>
@@ -2445,20 +2491,20 @@
       <c r="F10" s="22">
         <v>25.16</v>
       </c>
-      <c r="G10" s="31">
-        <v>20.32</v>
-      </c>
-      <c r="H10" s="28">
-        <v>16.46</v>
-      </c>
-      <c r="I10" s="5">
-        <v>16.46</v>
-      </c>
-      <c r="J10" s="25">
-        <v>67.370000000000104</v>
-      </c>
-      <c r="K10" s="19">
-        <v>25.16</v>
+      <c r="G10" s="41">
+        <v>0</v>
+      </c>
+      <c r="H10" s="39">
+        <v>0</v>
+      </c>
+      <c r="I10" s="39">
+        <v>0</v>
+      </c>
+      <c r="J10" s="39">
+        <v>0</v>
+      </c>
+      <c r="K10" s="40">
+        <v>0</v>
       </c>
       <c r="L10" s="34">
         <v>21.32</v>
@@ -2600,20 +2646,20 @@
       <c r="F11" s="22">
         <v>21.65</v>
       </c>
-      <c r="G11" s="31">
-        <v>20.36</v>
-      </c>
-      <c r="H11" s="28">
-        <v>16.79</v>
-      </c>
-      <c r="I11" s="5">
-        <v>16.79</v>
-      </c>
-      <c r="J11" s="25">
-        <v>63.410000000000103</v>
-      </c>
-      <c r="K11" s="19">
-        <v>21.65</v>
+      <c r="G11" s="63">
+        <v>0</v>
+      </c>
+      <c r="H11" s="64">
+        <v>0</v>
+      </c>
+      <c r="I11" s="64">
+        <v>0</v>
+      </c>
+      <c r="J11" s="64">
+        <v>0</v>
+      </c>
+      <c r="K11" s="65">
+        <v>0</v>
       </c>
       <c r="L11" s="34">
         <v>21.36</v>
@@ -2770,7 +2816,7 @@
       <c r="K12" s="18">
         <v>18.139999999999901</v>
       </c>
-      <c r="L12" s="37">
+      <c r="L12" s="36">
         <v>0</v>
       </c>
       <c r="M12" s="37">
@@ -2782,7 +2828,7 @@
       <c r="O12" s="37">
         <v>0</v>
       </c>
-      <c r="P12" s="37">
+      <c r="P12" s="62">
         <v>0</v>
       </c>
       <c r="Q12" s="30">
@@ -2925,20 +2971,20 @@
       <c r="K13" s="19">
         <v>14.6299999999999</v>
       </c>
-      <c r="L13" s="34">
-        <v>21.44</v>
-      </c>
-      <c r="M13" s="28">
-        <v>70.210000000000093</v>
-      </c>
-      <c r="N13" s="5">
-        <v>17.45</v>
-      </c>
-      <c r="O13" s="25">
-        <v>55.490000000000101</v>
-      </c>
-      <c r="P13" s="22">
-        <v>14.6299999999999</v>
+      <c r="L13" s="41">
+        <v>0</v>
+      </c>
+      <c r="M13" s="39">
+        <v>0</v>
+      </c>
+      <c r="N13" s="39">
+        <v>0</v>
+      </c>
+      <c r="O13" s="39">
+        <v>0</v>
+      </c>
+      <c r="P13" s="40">
+        <v>0</v>
       </c>
       <c r="Q13" s="31">
         <v>22.44</v>
@@ -3080,20 +3126,20 @@
       <c r="K14" s="19">
         <v>11.1199999999999</v>
       </c>
-      <c r="L14" s="34">
-        <v>21.48</v>
-      </c>
-      <c r="M14" s="28">
-        <v>70.330000000000098</v>
-      </c>
-      <c r="N14" s="5">
-        <v>17.78</v>
-      </c>
-      <c r="O14" s="25">
-        <v>51.530000000000101</v>
-      </c>
-      <c r="P14" s="22">
-        <v>11.1199999999999</v>
+      <c r="L14" s="41">
+        <v>0</v>
+      </c>
+      <c r="M14" s="39">
+        <v>0</v>
+      </c>
+      <c r="N14" s="39">
+        <v>0</v>
+      </c>
+      <c r="O14" s="39">
+        <v>0</v>
+      </c>
+      <c r="P14" s="40">
+        <v>0</v>
       </c>
       <c r="Q14" s="31">
         <v>22.48</v>
@@ -3235,20 +3281,20 @@
       <c r="K15" s="19">
         <v>7.6099999999999</v>
       </c>
-      <c r="L15" s="34">
-        <v>21.52</v>
-      </c>
-      <c r="M15" s="28">
-        <v>70.450000000000102</v>
-      </c>
-      <c r="N15" s="5">
-        <v>18.11</v>
-      </c>
-      <c r="O15" s="25">
-        <v>47.5700000000001</v>
-      </c>
-      <c r="P15" s="22">
-        <v>7.6099999999999</v>
+      <c r="L15" s="41">
+        <v>0</v>
+      </c>
+      <c r="M15" s="39">
+        <v>0</v>
+      </c>
+      <c r="N15" s="39">
+        <v>0</v>
+      </c>
+      <c r="O15" s="39">
+        <v>0</v>
+      </c>
+      <c r="P15" s="40">
+        <v>0</v>
       </c>
       <c r="Q15" s="31">
         <v>22.52</v>
@@ -3390,20 +3436,20 @@
       <c r="K16" s="20">
         <v>4.0999999999999002</v>
       </c>
-      <c r="L16" s="35">
-        <v>21.56</v>
-      </c>
-      <c r="M16" s="29">
-        <v>70.570000000000107</v>
-      </c>
-      <c r="N16" s="6">
-        <v>18.440000000000001</v>
-      </c>
-      <c r="O16" s="26">
-        <v>43.610000000000099</v>
-      </c>
-      <c r="P16" s="23">
-        <v>4.0999999999999002</v>
+      <c r="L16" s="63">
+        <v>0</v>
+      </c>
+      <c r="M16" s="64">
+        <v>0</v>
+      </c>
+      <c r="N16" s="64">
+        <v>0</v>
+      </c>
+      <c r="O16" s="64">
+        <v>0</v>
+      </c>
+      <c r="P16" s="65">
+        <v>0</v>
       </c>
       <c r="Q16" s="32">
         <v>22.56</v>
@@ -3560,19 +3606,19 @@
       <c r="P17" s="22">
         <v>0.58999999999990405</v>
       </c>
-      <c r="Q17" s="41">
-        <v>0</v>
-      </c>
-      <c r="R17" s="39">
-        <v>0</v>
-      </c>
-      <c r="S17" s="39">
-        <v>0</v>
-      </c>
-      <c r="T17" s="39">
-        <v>0</v>
-      </c>
-      <c r="U17" s="40">
+      <c r="Q17" s="36">
+        <v>0</v>
+      </c>
+      <c r="R17" s="37">
+        <v>0</v>
+      </c>
+      <c r="S17" s="37">
+        <v>0</v>
+      </c>
+      <c r="T17" s="37">
+        <v>0</v>
+      </c>
+      <c r="U17" s="62">
         <v>0</v>
       </c>
       <c r="V17" s="34">
@@ -3715,20 +3761,20 @@
       <c r="P18" s="22">
         <v>2.92</v>
       </c>
-      <c r="Q18" s="31">
-        <v>22.64</v>
-      </c>
-      <c r="R18" s="28">
-        <v>70.810000000000102</v>
-      </c>
-      <c r="S18" s="5">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="T18" s="25">
-        <v>35.690000000000097</v>
-      </c>
-      <c r="U18" s="19">
-        <v>2.92</v>
+      <c r="Q18" s="41">
+        <v>0</v>
+      </c>
+      <c r="R18" s="39">
+        <v>0</v>
+      </c>
+      <c r="S18" s="39">
+        <v>0</v>
+      </c>
+      <c r="T18" s="39">
+        <v>0</v>
+      </c>
+      <c r="U18" s="40">
+        <v>0</v>
       </c>
       <c r="V18" s="34">
         <v>23.64</v>
@@ -3870,20 +3916,20 @@
       <c r="P19" s="22">
         <v>6.43</v>
       </c>
-      <c r="Q19" s="31">
-        <v>22.68</v>
-      </c>
-      <c r="R19" s="28">
-        <v>70.930000000000106</v>
-      </c>
-      <c r="S19" s="5">
-        <v>19.43</v>
-      </c>
-      <c r="T19" s="25">
-        <v>31.7300000000001</v>
-      </c>
-      <c r="U19" s="19">
-        <v>6.43</v>
+      <c r="Q19" s="41">
+        <v>0</v>
+      </c>
+      <c r="R19" s="39">
+        <v>0</v>
+      </c>
+      <c r="S19" s="39">
+        <v>0</v>
+      </c>
+      <c r="T19" s="39">
+        <v>0</v>
+      </c>
+      <c r="U19" s="40">
+        <v>0</v>
       </c>
       <c r="V19" s="34">
         <v>23.68</v>
@@ -4025,20 +4071,20 @@
       <c r="P20" s="22">
         <v>9.94</v>
       </c>
-      <c r="Q20" s="31">
-        <v>22.72</v>
-      </c>
-      <c r="R20" s="28">
-        <v>71.050000000000097</v>
-      </c>
-      <c r="S20" s="5">
-        <v>19.760000000000002</v>
-      </c>
-      <c r="T20" s="25">
-        <v>27.770000000000099</v>
-      </c>
-      <c r="U20" s="19">
-        <v>9.94</v>
+      <c r="Q20" s="41">
+        <v>0</v>
+      </c>
+      <c r="R20" s="39">
+        <v>0</v>
+      </c>
+      <c r="S20" s="39">
+        <v>0</v>
+      </c>
+      <c r="T20" s="39">
+        <v>0</v>
+      </c>
+      <c r="U20" s="40">
+        <v>0</v>
       </c>
       <c r="V20" s="34">
         <v>23.72</v>
@@ -4180,20 +4226,20 @@
       <c r="P21" s="22">
         <v>13.45</v>
       </c>
-      <c r="Q21" s="31">
-        <v>22.76</v>
-      </c>
-      <c r="R21" s="28">
-        <v>71.170000000000101</v>
-      </c>
-      <c r="S21" s="5">
-        <v>20.09</v>
-      </c>
-      <c r="T21" s="25">
-        <v>23.810000000000102</v>
-      </c>
-      <c r="U21" s="19">
-        <v>13.45</v>
+      <c r="Q21" s="63">
+        <v>0</v>
+      </c>
+      <c r="R21" s="64">
+        <v>0</v>
+      </c>
+      <c r="S21" s="64">
+        <v>0</v>
+      </c>
+      <c r="T21" s="64">
+        <v>0</v>
+      </c>
+      <c r="U21" s="65">
+        <v>0</v>
       </c>
       <c r="V21" s="34">
         <v>23.76</v>
@@ -4350,7 +4396,7 @@
       <c r="U22" s="18">
         <v>16.96</v>
       </c>
-      <c r="V22" s="37">
+      <c r="V22" s="36">
         <v>0</v>
       </c>
       <c r="W22" s="37">
@@ -4362,7 +4408,7 @@
       <c r="Y22" s="37">
         <v>0</v>
       </c>
-      <c r="Z22" s="37">
+      <c r="Z22" s="62">
         <v>0</v>
       </c>
       <c r="AA22" s="30">
@@ -4505,20 +4551,20 @@
       <c r="U23" s="19">
         <v>20.47</v>
       </c>
-      <c r="V23" s="34">
-        <v>23.84</v>
-      </c>
-      <c r="W23" s="28">
-        <v>71.410000000000096</v>
-      </c>
-      <c r="X23" s="5">
-        <v>20.75</v>
-      </c>
-      <c r="Y23" s="25">
-        <v>15.8900000000001</v>
-      </c>
-      <c r="Z23" s="22">
-        <v>20.47</v>
+      <c r="V23" s="41">
+        <v>0</v>
+      </c>
+      <c r="W23" s="39">
+        <v>0</v>
+      </c>
+      <c r="X23" s="39">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="40">
+        <v>0</v>
       </c>
       <c r="AA23" s="31">
         <v>24.84</v>
@@ -4660,20 +4706,20 @@
       <c r="U24" s="19">
         <v>23.98</v>
       </c>
-      <c r="V24" s="34">
-        <v>23.88</v>
-      </c>
-      <c r="W24" s="28">
-        <v>71.530000000000101</v>
-      </c>
-      <c r="X24" s="5">
-        <v>21.08</v>
-      </c>
-      <c r="Y24" s="25">
-        <v>11.930000000000099</v>
-      </c>
-      <c r="Z24" s="22">
-        <v>23.98</v>
+      <c r="V24" s="41">
+        <v>0</v>
+      </c>
+      <c r="W24" s="39">
+        <v>0</v>
+      </c>
+      <c r="X24" s="39">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="40">
+        <v>0</v>
       </c>
       <c r="AA24" s="31">
         <v>24.88</v>
@@ -4815,20 +4861,20 @@
       <c r="U25" s="19">
         <v>27.49</v>
       </c>
-      <c r="V25" s="34">
-        <v>23.92</v>
-      </c>
-      <c r="W25" s="28">
-        <v>71.650000000000105</v>
-      </c>
-      <c r="X25" s="5">
-        <v>21.41</v>
-      </c>
-      <c r="Y25" s="25">
-        <v>7.9700000000001001</v>
-      </c>
-      <c r="Z25" s="22">
-        <v>27.49</v>
+      <c r="V25" s="41">
+        <v>0</v>
+      </c>
+      <c r="W25" s="39">
+        <v>0</v>
+      </c>
+      <c r="X25" s="39">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="40">
+        <v>0</v>
       </c>
       <c r="AA25" s="31">
         <v>24.92</v>
@@ -4970,20 +5016,20 @@
       <c r="U26" s="20">
         <v>31</v>
       </c>
-      <c r="V26" s="35">
-        <v>23.96</v>
-      </c>
-      <c r="W26" s="29">
-        <v>71.770000000000095</v>
-      </c>
-      <c r="X26" s="6">
-        <v>21.74</v>
-      </c>
-      <c r="Y26" s="26">
-        <v>4.0100000000001996</v>
-      </c>
-      <c r="Z26" s="23">
-        <v>31</v>
+      <c r="V26" s="63">
+        <v>0</v>
+      </c>
+      <c r="W26" s="64">
+        <v>0</v>
+      </c>
+      <c r="X26" s="64">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="64">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="65">
+        <v>0</v>
       </c>
       <c r="AA26" s="32">
         <v>24.96</v>
@@ -5140,19 +5186,19 @@
       <c r="Z27" s="22">
         <v>34.51</v>
       </c>
-      <c r="AA27" s="41">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="39">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="39">
-        <v>0</v>
-      </c>
-      <c r="AD27" s="39">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="40">
+      <c r="AA27" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="37">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="37">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="37">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="62">
         <v>0</v>
       </c>
       <c r="AF27" s="34">
@@ -5295,20 +5341,20 @@
       <c r="Z28" s="22">
         <v>38.020000000000003</v>
       </c>
-      <c r="AA28" s="31">
-        <v>25.04</v>
-      </c>
-      <c r="AB28" s="28">
-        <v>72.010000000000105</v>
-      </c>
-      <c r="AC28" s="5">
-        <v>22.4</v>
-      </c>
-      <c r="AD28" s="25">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="AE28" s="19">
-        <v>38.020000000000003</v>
+      <c r="AA28" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="39">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="39">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="39">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="40">
+        <v>0</v>
       </c>
       <c r="AF28" s="34">
         <v>26.04</v>
@@ -5450,20 +5496,20 @@
       <c r="Z29" s="22">
         <v>41.53</v>
       </c>
-      <c r="AA29" s="31">
-        <v>25.08</v>
-      </c>
-      <c r="AB29" s="28">
-        <v>72.130000000000095</v>
-      </c>
-      <c r="AC29" s="5">
-        <v>22.73</v>
-      </c>
-      <c r="AD29" s="25">
-        <v>3.78</v>
-      </c>
-      <c r="AE29" s="19">
-        <v>41.53</v>
+      <c r="AA29" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="39">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="39">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="39">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="40">
+        <v>0</v>
       </c>
       <c r="AF29" s="34">
         <v>26.08</v>
@@ -5605,20 +5651,20 @@
       <c r="Z30" s="22">
         <v>45.04</v>
       </c>
-      <c r="AA30" s="31">
-        <v>25.12</v>
-      </c>
-      <c r="AB30" s="28">
-        <v>72.250000000000099</v>
-      </c>
-      <c r="AC30" s="5">
-        <v>23.06</v>
-      </c>
-      <c r="AD30" s="25">
-        <v>6.47</v>
-      </c>
-      <c r="AE30" s="19">
-        <v>45.04</v>
+      <c r="AA30" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="39">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="39">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="39">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="40">
+        <v>0</v>
       </c>
       <c r="AF30" s="34">
         <v>26.12</v>
@@ -5760,20 +5806,20 @@
       <c r="Z31" s="22">
         <v>48.55</v>
       </c>
-      <c r="AA31" s="31">
-        <v>25.16</v>
-      </c>
-      <c r="AB31" s="28">
-        <v>72.370000000000104</v>
-      </c>
-      <c r="AC31" s="5">
-        <v>23.39</v>
-      </c>
-      <c r="AD31" s="25">
-        <v>9.16</v>
-      </c>
-      <c r="AE31" s="19">
-        <v>48.55</v>
+      <c r="AA31" s="63">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="64">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="64">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="64">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="65">
+        <v>0</v>
       </c>
       <c r="AF31" s="34">
         <v>26.16</v>
@@ -5930,7 +5976,7 @@
       <c r="AE32" s="18">
         <v>52.06</v>
       </c>
-      <c r="AF32" s="37">
+      <c r="AF32" s="36">
         <v>0</v>
       </c>
       <c r="AG32" s="37">
@@ -5942,7 +5988,7 @@
       <c r="AI32" s="37">
         <v>0</v>
       </c>
-      <c r="AJ32" s="37">
+      <c r="AJ32" s="62">
         <v>0</v>
       </c>
       <c r="AK32" s="30">
@@ -6085,20 +6131,20 @@
       <c r="AE33" s="19">
         <v>55.57</v>
       </c>
-      <c r="AF33" s="34">
-        <v>26.24</v>
-      </c>
-      <c r="AG33" s="28">
-        <v>72.610000000000099</v>
-      </c>
-      <c r="AH33" s="5">
-        <v>24.05</v>
-      </c>
-      <c r="AI33" s="25">
-        <v>14.54</v>
-      </c>
-      <c r="AJ33" s="22">
-        <v>55.57</v>
+      <c r="AF33" s="41">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="39">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="39">
+        <v>0</v>
+      </c>
+      <c r="AI33" s="39">
+        <v>0</v>
+      </c>
+      <c r="AJ33" s="40">
+        <v>0</v>
       </c>
       <c r="AK33" s="31">
         <v>27.24</v>
@@ -6240,20 +6286,20 @@
       <c r="AE34" s="19">
         <v>59.08</v>
       </c>
-      <c r="AF34" s="34">
-        <v>26.28</v>
-      </c>
-      <c r="AG34" s="28">
-        <v>72.730000000000103</v>
-      </c>
-      <c r="AH34" s="5">
-        <v>24.38</v>
-      </c>
-      <c r="AI34" s="25">
-        <v>17.23</v>
-      </c>
-      <c r="AJ34" s="22">
-        <v>59.08</v>
+      <c r="AF34" s="41">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="39">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="39">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="39">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="40">
+        <v>0</v>
       </c>
       <c r="AK34" s="31">
         <v>27.28</v>
@@ -6395,20 +6441,20 @@
       <c r="AE35" s="19">
         <v>62.59</v>
       </c>
-      <c r="AF35" s="34">
-        <v>26.32</v>
-      </c>
-      <c r="AG35" s="28">
-        <v>72.850000000000193</v>
-      </c>
-      <c r="AH35" s="5">
-        <v>24.71</v>
-      </c>
-      <c r="AI35" s="25">
-        <v>19.920000000000002</v>
-      </c>
-      <c r="AJ35" s="22">
-        <v>62.59</v>
+      <c r="AF35" s="41">
+        <v>0</v>
+      </c>
+      <c r="AG35" s="39">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="39">
+        <v>0</v>
+      </c>
+      <c r="AI35" s="39">
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="40">
+        <v>0</v>
       </c>
       <c r="AK35" s="31">
         <v>27.32</v>
@@ -6550,20 +6596,20 @@
       <c r="AE36" s="20">
         <v>66.099999999999994</v>
       </c>
-      <c r="AF36" s="35">
-        <v>26.36</v>
-      </c>
-      <c r="AG36" s="29">
-        <v>72.970000000000198</v>
-      </c>
-      <c r="AH36" s="6">
-        <v>25.04</v>
-      </c>
-      <c r="AI36" s="26">
-        <v>22.61</v>
-      </c>
-      <c r="AJ36" s="23">
-        <v>66.099999999999994</v>
+      <c r="AF36" s="63">
+        <v>0</v>
+      </c>
+      <c r="AG36" s="64">
+        <v>0</v>
+      </c>
+      <c r="AH36" s="64">
+        <v>0</v>
+      </c>
+      <c r="AI36" s="64">
+        <v>0</v>
+      </c>
+      <c r="AJ36" s="65">
+        <v>0</v>
       </c>
       <c r="AK36" s="32">
         <v>27.36</v>
@@ -6720,19 +6766,19 @@
       <c r="AJ37" s="22">
         <v>69.61</v>
       </c>
-      <c r="AK37" s="41">
-        <v>0</v>
-      </c>
-      <c r="AL37" s="39">
-        <v>0</v>
-      </c>
-      <c r="AM37" s="39">
-        <v>0</v>
-      </c>
-      <c r="AN37" s="39">
-        <v>0</v>
-      </c>
-      <c r="AO37" s="40">
+      <c r="AK37" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL37" s="37">
+        <v>0</v>
+      </c>
+      <c r="AM37" s="37">
+        <v>0</v>
+      </c>
+      <c r="AN37" s="37">
+        <v>0</v>
+      </c>
+      <c r="AO37" s="62">
         <v>0</v>
       </c>
       <c r="AP37" s="34">
@@ -6875,20 +6921,20 @@
       <c r="AJ38" s="22">
         <v>73.12</v>
       </c>
-      <c r="AK38" s="31">
-        <v>27.44</v>
-      </c>
-      <c r="AL38" s="28">
-        <v>73.210000000000207</v>
-      </c>
-      <c r="AM38" s="5">
-        <v>25.7</v>
-      </c>
-      <c r="AN38" s="25">
-        <v>27.99</v>
-      </c>
-      <c r="AO38" s="19">
-        <v>73.12</v>
+      <c r="AK38" s="41">
+        <v>0</v>
+      </c>
+      <c r="AL38" s="39">
+        <v>0</v>
+      </c>
+      <c r="AM38" s="39">
+        <v>0</v>
+      </c>
+      <c r="AN38" s="39">
+        <v>0</v>
+      </c>
+      <c r="AO38" s="40">
+        <v>0</v>
       </c>
       <c r="AP38" s="34">
         <v>28.44</v>
@@ -7030,20 +7076,20 @@
       <c r="AJ39" s="22">
         <v>76.63</v>
       </c>
-      <c r="AK39" s="31">
-        <v>27.48</v>
-      </c>
-      <c r="AL39" s="28">
-        <v>73.330000000000197</v>
-      </c>
-      <c r="AM39" s="5">
-        <v>26.03</v>
-      </c>
-      <c r="AN39" s="25">
-        <v>30.68</v>
-      </c>
-      <c r="AO39" s="19">
-        <v>76.63</v>
+      <c r="AK39" s="41">
+        <v>0</v>
+      </c>
+      <c r="AL39" s="39">
+        <v>0</v>
+      </c>
+      <c r="AM39" s="39">
+        <v>0</v>
+      </c>
+      <c r="AN39" s="39">
+        <v>0</v>
+      </c>
+      <c r="AO39" s="40">
+        <v>0</v>
       </c>
       <c r="AP39" s="34">
         <v>28.48</v>
@@ -7185,20 +7231,20 @@
       <c r="AJ40" s="22">
         <v>80.14</v>
       </c>
-      <c r="AK40" s="31">
-        <v>27.52</v>
-      </c>
-      <c r="AL40" s="28">
-        <v>73.450000000000202</v>
-      </c>
-      <c r="AM40" s="5">
-        <v>26.36</v>
-      </c>
-      <c r="AN40" s="25">
-        <v>33.369999999999997</v>
-      </c>
-      <c r="AO40" s="19">
-        <v>80.14</v>
+      <c r="AK40" s="41">
+        <v>0</v>
+      </c>
+      <c r="AL40" s="39">
+        <v>0</v>
+      </c>
+      <c r="AM40" s="39">
+        <v>0</v>
+      </c>
+      <c r="AN40" s="39">
+        <v>0</v>
+      </c>
+      <c r="AO40" s="40">
+        <v>0</v>
       </c>
       <c r="AP40" s="34">
         <v>28.52</v>
@@ -7340,20 +7386,20 @@
       <c r="AJ41" s="22">
         <v>83.65</v>
       </c>
-      <c r="AK41" s="31">
-        <v>27.56</v>
-      </c>
-      <c r="AL41" s="28">
-        <v>73.570000000000206</v>
-      </c>
-      <c r="AM41" s="5">
-        <v>26.69</v>
-      </c>
-      <c r="AN41" s="25">
-        <v>36.06</v>
-      </c>
-      <c r="AO41" s="19">
-        <v>83.65</v>
+      <c r="AK41" s="63">
+        <v>0</v>
+      </c>
+      <c r="AL41" s="64">
+        <v>0</v>
+      </c>
+      <c r="AM41" s="64">
+        <v>0</v>
+      </c>
+      <c r="AN41" s="64">
+        <v>0</v>
+      </c>
+      <c r="AO41" s="65">
+        <v>0</v>
       </c>
       <c r="AP41" s="34">
         <v>28.56</v>
@@ -7510,7 +7556,7 @@
       <c r="AO42" s="18">
         <v>87.16</v>
       </c>
-      <c r="AP42" s="37">
+      <c r="AP42" s="36">
         <v>0</v>
       </c>
       <c r="AQ42" s="37">
@@ -7522,7 +7568,7 @@
       <c r="AS42" s="37">
         <v>0</v>
       </c>
-      <c r="AT42" s="37">
+      <c r="AT42" s="62">
         <v>0</v>
       </c>
       <c r="AU42" s="30">
@@ -7665,20 +7711,20 @@
       <c r="AO43" s="19">
         <v>90.67</v>
       </c>
-      <c r="AP43" s="34">
-        <v>28.64</v>
-      </c>
-      <c r="AQ43" s="28">
-        <v>73.810000000000201</v>
-      </c>
-      <c r="AR43" s="5">
-        <v>27.35</v>
-      </c>
-      <c r="AS43" s="25">
-        <v>41.44</v>
-      </c>
-      <c r="AT43" s="22">
-        <v>90.67</v>
+      <c r="AP43" s="41">
+        <v>0</v>
+      </c>
+      <c r="AQ43" s="39">
+        <v>0</v>
+      </c>
+      <c r="AR43" s="39">
+        <v>0</v>
+      </c>
+      <c r="AS43" s="39">
+        <v>0</v>
+      </c>
+      <c r="AT43" s="40">
+        <v>0</v>
       </c>
       <c r="AU43" s="31">
         <v>29.64</v>
@@ -7820,20 +7866,20 @@
       <c r="AO44" s="19">
         <v>94.18</v>
       </c>
-      <c r="AP44" s="34">
-        <v>28.68</v>
-      </c>
-      <c r="AQ44" s="28">
-        <v>73.930000000000206</v>
-      </c>
-      <c r="AR44" s="5">
-        <v>27.68</v>
-      </c>
-      <c r="AS44" s="25">
-        <v>44.13</v>
-      </c>
-      <c r="AT44" s="22">
-        <v>94.18</v>
+      <c r="AP44" s="41">
+        <v>0</v>
+      </c>
+      <c r="AQ44" s="39">
+        <v>0</v>
+      </c>
+      <c r="AR44" s="39">
+        <v>0</v>
+      </c>
+      <c r="AS44" s="39">
+        <v>0</v>
+      </c>
+      <c r="AT44" s="40">
+        <v>0</v>
       </c>
       <c r="AU44" s="31">
         <v>29.68</v>
@@ -7975,20 +8021,20 @@
       <c r="AO45" s="19">
         <v>97.69</v>
       </c>
-      <c r="AP45" s="34">
-        <v>28.72</v>
-      </c>
-      <c r="AQ45" s="28">
-        <v>74.050000000000196</v>
-      </c>
-      <c r="AR45" s="5">
-        <v>28.01</v>
-      </c>
-      <c r="AS45" s="25">
-        <v>46.82</v>
-      </c>
-      <c r="AT45" s="22">
-        <v>97.69</v>
+      <c r="AP45" s="41">
+        <v>0</v>
+      </c>
+      <c r="AQ45" s="39">
+        <v>0</v>
+      </c>
+      <c r="AR45" s="39">
+        <v>0</v>
+      </c>
+      <c r="AS45" s="39">
+        <v>0</v>
+      </c>
+      <c r="AT45" s="40">
+        <v>0</v>
       </c>
       <c r="AU45" s="31">
         <v>29.72</v>
@@ -8130,20 +8176,20 @@
       <c r="AO46" s="20">
         <v>1.02</v>
       </c>
-      <c r="AP46" s="35">
-        <v>28.76</v>
-      </c>
-      <c r="AQ46" s="29">
-        <v>74.170000000000201</v>
-      </c>
-      <c r="AR46" s="6">
-        <v>28.34</v>
-      </c>
-      <c r="AS46" s="26">
-        <v>49.51</v>
-      </c>
-      <c r="AT46" s="23">
-        <v>1.02</v>
+      <c r="AP46" s="63">
+        <v>0</v>
+      </c>
+      <c r="AQ46" s="64">
+        <v>0</v>
+      </c>
+      <c r="AR46" s="64">
+        <v>0</v>
+      </c>
+      <c r="AS46" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT46" s="65">
+        <v>0</v>
       </c>
       <c r="AU46" s="32">
         <v>29.76</v>
@@ -8300,19 +8346,19 @@
       <c r="AT47" s="22">
         <v>4.71</v>
       </c>
-      <c r="AU47" s="41">
-        <v>0</v>
-      </c>
-      <c r="AV47" s="39">
-        <v>0</v>
-      </c>
-      <c r="AW47" s="39">
-        <v>0</v>
-      </c>
-      <c r="AX47" s="39">
-        <v>0</v>
-      </c>
-      <c r="AY47" s="40">
+      <c r="AU47" s="36">
+        <v>0</v>
+      </c>
+      <c r="AV47" s="37">
+        <v>0</v>
+      </c>
+      <c r="AW47" s="37">
+        <v>0</v>
+      </c>
+      <c r="AX47" s="37">
+        <v>0</v>
+      </c>
+      <c r="AY47" s="62">
         <v>0</v>
       </c>
     </row>
@@ -8455,20 +8501,20 @@
       <c r="AT48" s="22">
         <v>8.4</v>
       </c>
-      <c r="AU48" s="31">
-        <v>29.84</v>
-      </c>
-      <c r="AV48" s="28">
-        <v>74.410000000000196</v>
-      </c>
-      <c r="AW48" s="5">
-        <v>29</v>
-      </c>
-      <c r="AX48" s="25">
-        <v>54.89</v>
-      </c>
-      <c r="AY48" s="19">
-        <v>8.4</v>
+      <c r="AU48" s="41">
+        <v>0</v>
+      </c>
+      <c r="AV48" s="39">
+        <v>0</v>
+      </c>
+      <c r="AW48" s="39">
+        <v>0</v>
+      </c>
+      <c r="AX48" s="39">
+        <v>0</v>
+      </c>
+      <c r="AY48" s="40">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:51" x14ac:dyDescent="0.25">
@@ -8610,20 +8656,20 @@
       <c r="AT49" s="22">
         <v>12.09</v>
       </c>
-      <c r="AU49" s="31">
-        <v>29.88</v>
-      </c>
-      <c r="AV49" s="28">
-        <v>74.5300000000002</v>
-      </c>
-      <c r="AW49" s="5">
-        <v>29.33</v>
-      </c>
-      <c r="AX49" s="25">
-        <v>57.58</v>
-      </c>
-      <c r="AY49" s="19">
-        <v>12.09</v>
+      <c r="AU49" s="41">
+        <v>0</v>
+      </c>
+      <c r="AV49" s="39">
+        <v>0</v>
+      </c>
+      <c r="AW49" s="39">
+        <v>0</v>
+      </c>
+      <c r="AX49" s="39">
+        <v>0</v>
+      </c>
+      <c r="AY49" s="40">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:51" x14ac:dyDescent="0.25">
@@ -8765,20 +8811,20 @@
       <c r="AT50" s="22">
         <v>15.78</v>
       </c>
-      <c r="AU50" s="31">
-        <v>29.92</v>
-      </c>
-      <c r="AV50" s="28">
-        <v>74.650000000000205</v>
-      </c>
-      <c r="AW50" s="5">
-        <v>29.66</v>
-      </c>
-      <c r="AX50" s="25">
-        <v>60.27</v>
-      </c>
-      <c r="AY50" s="19">
-        <v>15.78</v>
+      <c r="AU50" s="41">
+        <v>0</v>
+      </c>
+      <c r="AV50" s="39">
+        <v>0</v>
+      </c>
+      <c r="AW50" s="39">
+        <v>0</v>
+      </c>
+      <c r="AX50" s="39">
+        <v>0</v>
+      </c>
+      <c r="AY50" s="40">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:51" x14ac:dyDescent="0.25">
@@ -8920,20 +8966,20 @@
       <c r="AT51" s="23">
         <v>19.47</v>
       </c>
-      <c r="AU51" s="32">
-        <v>29.96</v>
-      </c>
-      <c r="AV51" s="29">
-        <v>74.770000000000195</v>
-      </c>
-      <c r="AW51" s="6">
-        <v>29.99</v>
-      </c>
-      <c r="AX51" s="26">
-        <v>62.96</v>
-      </c>
-      <c r="AY51" s="20">
-        <v>19.47</v>
+      <c r="AU51" s="63">
+        <v>0</v>
+      </c>
+      <c r="AV51" s="64">
+        <v>0</v>
+      </c>
+      <c r="AW51" s="64">
+        <v>0</v>
+      </c>
+      <c r="AX51" s="64">
+        <v>0</v>
+      </c>
+      <c r="AY51" s="65">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8947,7 +8993,7 @@
   <dimension ref="A1:AY51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="AP37" sqref="AP37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9127,10 +9173,10 @@
       <c r="E2" s="37">
         <v>0</v>
       </c>
-      <c r="F2" s="37">
-        <v>0</v>
-      </c>
-      <c r="G2" s="30">
+      <c r="F2" s="62">
+        <v>0</v>
+      </c>
+      <c r="G2" s="33">
         <v>20</v>
       </c>
       <c r="H2" s="27">
@@ -9270,22 +9316,22 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31">
-        <v>20.04</v>
-      </c>
-      <c r="C3" s="28">
-        <v>69.12</v>
-      </c>
-      <c r="D3" s="5">
-        <v>14.15</v>
-      </c>
-      <c r="E3" s="25">
-        <v>95.09</v>
-      </c>
-      <c r="F3" s="22">
-        <v>49.73</v>
-      </c>
-      <c r="G3" s="31">
+      <c r="B3" s="41">
+        <v>0</v>
+      </c>
+      <c r="C3" s="39">
+        <v>0</v>
+      </c>
+      <c r="D3" s="39">
+        <v>0</v>
+      </c>
+      <c r="E3" s="39">
+        <v>0</v>
+      </c>
+      <c r="F3" s="40">
+        <v>0</v>
+      </c>
+      <c r="G3" s="34">
         <v>20.04</v>
       </c>
       <c r="H3" s="28">
@@ -9425,22 +9471,22 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31">
-        <v>20.079999999999998</v>
-      </c>
-      <c r="C4" s="28">
-        <v>69.13</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="25">
-        <v>91.13</v>
-      </c>
-      <c r="F4" s="22">
-        <v>46.22</v>
-      </c>
-      <c r="G4" s="31">
+      <c r="B4" s="41">
+        <v>0</v>
+      </c>
+      <c r="C4" s="39">
+        <v>0</v>
+      </c>
+      <c r="D4" s="39">
+        <v>0</v>
+      </c>
+      <c r="E4" s="39">
+        <v>0</v>
+      </c>
+      <c r="F4" s="40">
+        <v>0</v>
+      </c>
+      <c r="G4" s="34">
         <v>20.079999999999998</v>
       </c>
       <c r="H4" s="28">
@@ -9580,22 +9626,22 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="31">
-        <v>20.12</v>
-      </c>
-      <c r="C5" s="28">
-        <v>69.25</v>
-      </c>
-      <c r="D5" s="5">
-        <v>14.81</v>
-      </c>
-      <c r="E5" s="25">
-        <v>0</v>
-      </c>
-      <c r="F5" s="22">
-        <v>42.71</v>
-      </c>
-      <c r="G5" s="31">
+      <c r="B5" s="41">
+        <v>0</v>
+      </c>
+      <c r="C5" s="39">
+        <v>0</v>
+      </c>
+      <c r="D5" s="39">
+        <v>0</v>
+      </c>
+      <c r="E5" s="39">
+        <v>0</v>
+      </c>
+      <c r="F5" s="40">
+        <v>0</v>
+      </c>
+      <c r="G5" s="34">
         <v>20.12</v>
       </c>
       <c r="H5" s="28">
@@ -9735,22 +9781,22 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="32">
-        <v>20.16</v>
-      </c>
-      <c r="C6" s="29">
-        <v>69.37</v>
-      </c>
-      <c r="D6" s="6">
-        <v>15.14</v>
-      </c>
-      <c r="E6" s="26">
-        <v>83.21</v>
-      </c>
-      <c r="F6" s="23">
-        <v>39.200000000000003</v>
-      </c>
-      <c r="G6" s="32">
+      <c r="B6" s="63">
+        <v>0</v>
+      </c>
+      <c r="C6" s="64">
+        <v>0</v>
+      </c>
+      <c r="D6" s="64">
+        <v>0</v>
+      </c>
+      <c r="E6" s="64">
+        <v>0</v>
+      </c>
+      <c r="F6" s="65">
+        <v>0</v>
+      </c>
+      <c r="G6" s="35">
         <v>20.16</v>
       </c>
       <c r="H6" s="29">
@@ -9905,19 +9951,19 @@
       <c r="F7" s="22">
         <v>35.69</v>
       </c>
-      <c r="G7" s="41">
-        <v>0</v>
-      </c>
-      <c r="H7" s="39">
-        <v>0</v>
-      </c>
-      <c r="I7" s="39">
-        <v>0</v>
-      </c>
-      <c r="J7" s="39">
-        <v>0</v>
-      </c>
-      <c r="K7" s="40">
+      <c r="G7" s="36">
+        <v>0</v>
+      </c>
+      <c r="H7" s="37">
+        <v>0</v>
+      </c>
+      <c r="I7" s="37">
+        <v>0</v>
+      </c>
+      <c r="J7" s="37">
+        <v>0</v>
+      </c>
+      <c r="K7" s="62">
         <v>0</v>
       </c>
       <c r="L7" s="34">
@@ -10060,20 +10106,20 @@
       <c r="F8" s="22">
         <v>32.18</v>
       </c>
-      <c r="G8" s="31">
-        <v>20.239999999999998</v>
-      </c>
-      <c r="H8" s="28">
-        <v>15.8</v>
-      </c>
-      <c r="I8" s="5">
-        <v>15.8</v>
-      </c>
-      <c r="J8" s="25">
-        <v>75.290000000000006</v>
-      </c>
-      <c r="K8" s="19">
-        <v>32.18</v>
+      <c r="G8" s="41">
+        <v>0</v>
+      </c>
+      <c r="H8" s="39">
+        <v>0</v>
+      </c>
+      <c r="I8" s="39">
+        <v>0</v>
+      </c>
+      <c r="J8" s="39">
+        <v>0</v>
+      </c>
+      <c r="K8" s="40">
+        <v>0</v>
       </c>
       <c r="L8" s="34">
         <v>21.24</v>
@@ -10215,20 +10261,20 @@
       <c r="F9" s="22">
         <v>28.67</v>
       </c>
-      <c r="G9" s="31">
-        <v>20.28</v>
-      </c>
-      <c r="H9" s="28">
-        <v>16.13</v>
-      </c>
-      <c r="I9" s="5">
-        <v>16.13</v>
-      </c>
-      <c r="J9" s="25">
-        <v>71.33</v>
-      </c>
-      <c r="K9" s="19">
-        <v>28.67</v>
+      <c r="G9" s="41">
+        <v>0</v>
+      </c>
+      <c r="H9" s="39">
+        <v>0</v>
+      </c>
+      <c r="I9" s="39">
+        <v>0</v>
+      </c>
+      <c r="J9" s="39">
+        <v>0</v>
+      </c>
+      <c r="K9" s="40">
+        <v>0</v>
       </c>
       <c r="L9" s="34">
         <v>21.28</v>
@@ -10370,20 +10416,20 @@
       <c r="F10" s="22">
         <v>25.16</v>
       </c>
-      <c r="G10" s="31">
-        <v>20.32</v>
-      </c>
-      <c r="H10" s="28">
-        <v>16.46</v>
-      </c>
-      <c r="I10" s="5">
-        <v>16.46</v>
-      </c>
-      <c r="J10" s="25">
-        <v>67.370000000000104</v>
-      </c>
-      <c r="K10" s="19">
-        <v>25.16</v>
+      <c r="G10" s="41">
+        <v>0</v>
+      </c>
+      <c r="H10" s="39">
+        <v>0</v>
+      </c>
+      <c r="I10" s="39">
+        <v>0</v>
+      </c>
+      <c r="J10" s="39">
+        <v>0</v>
+      </c>
+      <c r="K10" s="40">
+        <v>0</v>
       </c>
       <c r="L10" s="34">
         <v>21.32</v>
@@ -10525,20 +10571,20 @@
       <c r="F11" s="22">
         <v>21.65</v>
       </c>
-      <c r="G11" s="31">
-        <v>20.36</v>
-      </c>
-      <c r="H11" s="28">
-        <v>16.79</v>
-      </c>
-      <c r="I11" s="5">
-        <v>16.79</v>
-      </c>
-      <c r="J11" s="25">
-        <v>63.410000000000103</v>
-      </c>
-      <c r="K11" s="19">
-        <v>21.65</v>
+      <c r="G11" s="63">
+        <v>0</v>
+      </c>
+      <c r="H11" s="64">
+        <v>0</v>
+      </c>
+      <c r="I11" s="64">
+        <v>0</v>
+      </c>
+      <c r="J11" s="64">
+        <v>0</v>
+      </c>
+      <c r="K11" s="65">
+        <v>0</v>
       </c>
       <c r="L11" s="34">
         <v>21.36</v>
@@ -10695,7 +10741,7 @@
       <c r="K12" s="18">
         <v>18.139999999999901</v>
       </c>
-      <c r="L12" s="37">
+      <c r="L12" s="36">
         <v>0</v>
       </c>
       <c r="M12" s="37">
@@ -10707,7 +10753,7 @@
       <c r="O12" s="37">
         <v>0</v>
       </c>
-      <c r="P12" s="37">
+      <c r="P12" s="62">
         <v>0</v>
       </c>
       <c r="Q12" s="30">
@@ -10850,20 +10896,20 @@
       <c r="K13" s="19">
         <v>14.6299999999999</v>
       </c>
-      <c r="L13" s="34">
-        <v>21.44</v>
-      </c>
-      <c r="M13" s="28">
-        <v>70.210000000000093</v>
-      </c>
-      <c r="N13" s="5">
-        <v>17.45</v>
-      </c>
-      <c r="O13" s="25">
-        <v>55.490000000000101</v>
-      </c>
-      <c r="P13" s="22">
-        <v>14.6299999999999</v>
+      <c r="L13" s="41">
+        <v>0</v>
+      </c>
+      <c r="M13" s="39">
+        <v>0</v>
+      </c>
+      <c r="N13" s="39">
+        <v>0</v>
+      </c>
+      <c r="O13" s="39">
+        <v>0</v>
+      </c>
+      <c r="P13" s="40">
+        <v>0</v>
       </c>
       <c r="Q13" s="31">
         <v>22.44</v>
@@ -11005,20 +11051,20 @@
       <c r="K14" s="19">
         <v>11.1199999999999</v>
       </c>
-      <c r="L14" s="34">
-        <v>21.48</v>
-      </c>
-      <c r="M14" s="28">
-        <v>70.330000000000098</v>
-      </c>
-      <c r="N14" s="5">
-        <v>17.78</v>
-      </c>
-      <c r="O14" s="25">
-        <v>51.530000000000101</v>
-      </c>
-      <c r="P14" s="22">
-        <v>11.1199999999999</v>
+      <c r="L14" s="41">
+        <v>0</v>
+      </c>
+      <c r="M14" s="39">
+        <v>0</v>
+      </c>
+      <c r="N14" s="39">
+        <v>0</v>
+      </c>
+      <c r="O14" s="39">
+        <v>0</v>
+      </c>
+      <c r="P14" s="40">
+        <v>0</v>
       </c>
       <c r="Q14" s="31">
         <v>22.48</v>
@@ -11160,20 +11206,20 @@
       <c r="K15" s="19">
         <v>7.6099999999999</v>
       </c>
-      <c r="L15" s="34">
-        <v>21.52</v>
-      </c>
-      <c r="M15" s="28">
-        <v>70.450000000000102</v>
-      </c>
-      <c r="N15" s="5">
-        <v>18.11</v>
-      </c>
-      <c r="O15" s="25">
-        <v>47.5700000000001</v>
-      </c>
-      <c r="P15" s="22">
-        <v>7.6099999999999</v>
+      <c r="L15" s="41">
+        <v>0</v>
+      </c>
+      <c r="M15" s="39">
+        <v>0</v>
+      </c>
+      <c r="N15" s="39">
+        <v>0</v>
+      </c>
+      <c r="O15" s="39">
+        <v>0</v>
+      </c>
+      <c r="P15" s="40">
+        <v>0</v>
       </c>
       <c r="Q15" s="31">
         <v>22.52</v>
@@ -11315,20 +11361,20 @@
       <c r="K16" s="20">
         <v>4.0999999999999002</v>
       </c>
-      <c r="L16" s="35">
-        <v>21.56</v>
-      </c>
-      <c r="M16" s="29">
-        <v>70.570000000000107</v>
-      </c>
-      <c r="N16" s="6">
-        <v>18.440000000000001</v>
-      </c>
-      <c r="O16" s="26">
-        <v>43.610000000000099</v>
-      </c>
-      <c r="P16" s="23">
-        <v>4.0999999999999002</v>
+      <c r="L16" s="63">
+        <v>0</v>
+      </c>
+      <c r="M16" s="64">
+        <v>0</v>
+      </c>
+      <c r="N16" s="64">
+        <v>0</v>
+      </c>
+      <c r="O16" s="64">
+        <v>0</v>
+      </c>
+      <c r="P16" s="65">
+        <v>0</v>
       </c>
       <c r="Q16" s="32">
         <v>22.56</v>
@@ -11485,19 +11531,19 @@
       <c r="P17" s="22">
         <v>0.58999999999990405</v>
       </c>
-      <c r="Q17" s="41">
-        <v>0</v>
-      </c>
-      <c r="R17" s="39">
-        <v>0</v>
-      </c>
-      <c r="S17" s="39">
-        <v>0</v>
-      </c>
-      <c r="T17" s="39">
-        <v>0</v>
-      </c>
-      <c r="U17" s="40">
+      <c r="Q17" s="36">
+        <v>0</v>
+      </c>
+      <c r="R17" s="37">
+        <v>0</v>
+      </c>
+      <c r="S17" s="37">
+        <v>0</v>
+      </c>
+      <c r="T17" s="37">
+        <v>0</v>
+      </c>
+      <c r="U17" s="62">
         <v>0</v>
       </c>
       <c r="V17" s="34">
@@ -11640,20 +11686,20 @@
       <c r="P18" s="22">
         <v>2.92</v>
       </c>
-      <c r="Q18" s="31">
-        <v>22.64</v>
-      </c>
-      <c r="R18" s="28">
-        <v>70.810000000000102</v>
-      </c>
-      <c r="S18" s="5">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="T18" s="25">
-        <v>35.690000000000097</v>
-      </c>
-      <c r="U18" s="19">
-        <v>2.92</v>
+      <c r="Q18" s="41">
+        <v>0</v>
+      </c>
+      <c r="R18" s="39">
+        <v>0</v>
+      </c>
+      <c r="S18" s="39">
+        <v>0</v>
+      </c>
+      <c r="T18" s="39">
+        <v>0</v>
+      </c>
+      <c r="U18" s="40">
+        <v>0</v>
       </c>
       <c r="V18" s="34">
         <v>23.64</v>
@@ -11795,20 +11841,20 @@
       <c r="P19" s="22">
         <v>6.43</v>
       </c>
-      <c r="Q19" s="31">
-        <v>22.68</v>
-      </c>
-      <c r="R19" s="28">
-        <v>70.930000000000106</v>
-      </c>
-      <c r="S19" s="5">
-        <v>19.43</v>
-      </c>
-      <c r="T19" s="25">
-        <v>31.7300000000001</v>
-      </c>
-      <c r="U19" s="19">
-        <v>6.43</v>
+      <c r="Q19" s="41">
+        <v>0</v>
+      </c>
+      <c r="R19" s="39">
+        <v>0</v>
+      </c>
+      <c r="S19" s="39">
+        <v>0</v>
+      </c>
+      <c r="T19" s="39">
+        <v>0</v>
+      </c>
+      <c r="U19" s="40">
+        <v>0</v>
       </c>
       <c r="V19" s="34">
         <v>23.68</v>
@@ -11950,20 +11996,20 @@
       <c r="P20" s="22">
         <v>9.94</v>
       </c>
-      <c r="Q20" s="31">
-        <v>22.72</v>
-      </c>
-      <c r="R20" s="28">
-        <v>71.050000000000097</v>
-      </c>
-      <c r="S20" s="5">
-        <v>19.760000000000002</v>
-      </c>
-      <c r="T20" s="25">
-        <v>27.770000000000099</v>
-      </c>
-      <c r="U20" s="19">
-        <v>9.94</v>
+      <c r="Q20" s="41">
+        <v>0</v>
+      </c>
+      <c r="R20" s="39">
+        <v>0</v>
+      </c>
+      <c r="S20" s="39">
+        <v>0</v>
+      </c>
+      <c r="T20" s="39">
+        <v>0</v>
+      </c>
+      <c r="U20" s="40">
+        <v>0</v>
       </c>
       <c r="V20" s="34">
         <v>23.72</v>
@@ -12105,20 +12151,20 @@
       <c r="P21" s="22">
         <v>13.45</v>
       </c>
-      <c r="Q21" s="31">
-        <v>22.76</v>
-      </c>
-      <c r="R21" s="28">
-        <v>71.170000000000101</v>
-      </c>
-      <c r="S21" s="5">
-        <v>20.09</v>
-      </c>
-      <c r="T21" s="25">
-        <v>23.810000000000102</v>
-      </c>
-      <c r="U21" s="19">
-        <v>13.45</v>
+      <c r="Q21" s="63">
+        <v>0</v>
+      </c>
+      <c r="R21" s="64">
+        <v>0</v>
+      </c>
+      <c r="S21" s="64">
+        <v>0</v>
+      </c>
+      <c r="T21" s="64">
+        <v>0</v>
+      </c>
+      <c r="U21" s="65">
+        <v>0</v>
       </c>
       <c r="V21" s="34">
         <v>23.76</v>
@@ -12275,7 +12321,7 @@
       <c r="U22" s="18">
         <v>16.96</v>
       </c>
-      <c r="V22" s="37">
+      <c r="V22" s="36">
         <v>0</v>
       </c>
       <c r="W22" s="37">
@@ -12287,7 +12333,7 @@
       <c r="Y22" s="37">
         <v>0</v>
       </c>
-      <c r="Z22" s="37">
+      <c r="Z22" s="62">
         <v>0</v>
       </c>
       <c r="AA22" s="30">
@@ -12430,20 +12476,20 @@
       <c r="U23" s="19">
         <v>20.47</v>
       </c>
-      <c r="V23" s="34">
-        <v>23.84</v>
-      </c>
-      <c r="W23" s="28">
-        <v>71.410000000000096</v>
-      </c>
-      <c r="X23" s="5">
-        <v>20.75</v>
-      </c>
-      <c r="Y23" s="25">
-        <v>15.8900000000001</v>
-      </c>
-      <c r="Z23" s="22">
-        <v>20.47</v>
+      <c r="V23" s="41">
+        <v>0</v>
+      </c>
+      <c r="W23" s="39">
+        <v>0</v>
+      </c>
+      <c r="X23" s="39">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="40">
+        <v>0</v>
       </c>
       <c r="AA23" s="31">
         <v>24.84</v>
@@ -12585,20 +12631,20 @@
       <c r="U24" s="19">
         <v>23.98</v>
       </c>
-      <c r="V24" s="34">
-        <v>23.88</v>
-      </c>
-      <c r="W24" s="28">
-        <v>71.530000000000101</v>
-      </c>
-      <c r="X24" s="5">
-        <v>21.08</v>
-      </c>
-      <c r="Y24" s="25">
-        <v>11.930000000000099</v>
-      </c>
-      <c r="Z24" s="22">
-        <v>23.98</v>
+      <c r="V24" s="41">
+        <v>0</v>
+      </c>
+      <c r="W24" s="39">
+        <v>0</v>
+      </c>
+      <c r="X24" s="39">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="40">
+        <v>0</v>
       </c>
       <c r="AA24" s="31">
         <v>24.88</v>
@@ -12740,20 +12786,20 @@
       <c r="U25" s="19">
         <v>27.49</v>
       </c>
-      <c r="V25" s="34">
-        <v>23.92</v>
-      </c>
-      <c r="W25" s="28">
-        <v>71.650000000000105</v>
-      </c>
-      <c r="X25" s="5">
-        <v>21.41</v>
-      </c>
-      <c r="Y25" s="25">
-        <v>7.9700000000001001</v>
-      </c>
-      <c r="Z25" s="22">
-        <v>27.49</v>
+      <c r="V25" s="41">
+        <v>0</v>
+      </c>
+      <c r="W25" s="39">
+        <v>0</v>
+      </c>
+      <c r="X25" s="39">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="40">
+        <v>0</v>
       </c>
       <c r="AA25" s="31">
         <v>24.92</v>
@@ -12895,20 +12941,20 @@
       <c r="U26" s="20">
         <v>31</v>
       </c>
-      <c r="V26" s="35">
-        <v>23.96</v>
-      </c>
-      <c r="W26" s="29">
-        <v>71.770000000000095</v>
-      </c>
-      <c r="X26" s="6">
-        <v>21.74</v>
-      </c>
-      <c r="Y26" s="26">
-        <v>4.0100000000001996</v>
-      </c>
-      <c r="Z26" s="23">
-        <v>31</v>
+      <c r="V26" s="63">
+        <v>0</v>
+      </c>
+      <c r="W26" s="64">
+        <v>0</v>
+      </c>
+      <c r="X26" s="64">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="64">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="65">
+        <v>0</v>
       </c>
       <c r="AA26" s="32">
         <v>24.96</v>
@@ -13065,19 +13111,19 @@
       <c r="Z27" s="22">
         <v>34.51</v>
       </c>
-      <c r="AA27" s="41">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="39">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="39">
-        <v>0</v>
-      </c>
-      <c r="AD27" s="39">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="40">
+      <c r="AA27" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="37">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="37">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="37">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="62">
         <v>0</v>
       </c>
       <c r="AF27" s="34">
@@ -13220,20 +13266,20 @@
       <c r="Z28" s="22">
         <v>38.020000000000003</v>
       </c>
-      <c r="AA28" s="31">
-        <v>25.04</v>
-      </c>
-      <c r="AB28" s="28">
-        <v>72.010000000000105</v>
-      </c>
-      <c r="AC28" s="5">
-        <v>22.4</v>
-      </c>
-      <c r="AD28" s="25">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="AE28" s="19">
-        <v>38.020000000000003</v>
+      <c r="AA28" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="39">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="39">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="39">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="40">
+        <v>0</v>
       </c>
       <c r="AF28" s="34">
         <v>26.04</v>
@@ -13375,20 +13421,20 @@
       <c r="Z29" s="22">
         <v>41.53</v>
       </c>
-      <c r="AA29" s="31">
-        <v>25.08</v>
-      </c>
-      <c r="AB29" s="28">
-        <v>72.130000000000095</v>
-      </c>
-      <c r="AC29" s="5">
-        <v>22.73</v>
-      </c>
-      <c r="AD29" s="25">
-        <v>3.78</v>
-      </c>
-      <c r="AE29" s="19">
-        <v>41.53</v>
+      <c r="AA29" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="39">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="39">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="39">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="40">
+        <v>0</v>
       </c>
       <c r="AF29" s="34">
         <v>26.08</v>
@@ -13530,20 +13576,20 @@
       <c r="Z30" s="22">
         <v>45.04</v>
       </c>
-      <c r="AA30" s="31">
-        <v>25.12</v>
-      </c>
-      <c r="AB30" s="28">
-        <v>72.250000000000099</v>
-      </c>
-      <c r="AC30" s="5">
-        <v>23.06</v>
-      </c>
-      <c r="AD30" s="25">
-        <v>6.47</v>
-      </c>
-      <c r="AE30" s="19">
-        <v>45.04</v>
+      <c r="AA30" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="39">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="39">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="39">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="40">
+        <v>0</v>
       </c>
       <c r="AF30" s="34">
         <v>26.12</v>
@@ -13685,20 +13731,20 @@
       <c r="Z31" s="22">
         <v>48.55</v>
       </c>
-      <c r="AA31" s="31">
-        <v>25.16</v>
-      </c>
-      <c r="AB31" s="28">
-        <v>72.370000000000104</v>
-      </c>
-      <c r="AC31" s="5">
-        <v>23.39</v>
-      </c>
-      <c r="AD31" s="25">
-        <v>9.16</v>
-      </c>
-      <c r="AE31" s="19">
-        <v>48.55</v>
+      <c r="AA31" s="63">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="64">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="64">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="64">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="65">
+        <v>0</v>
       </c>
       <c r="AF31" s="34">
         <v>26.16</v>
@@ -13855,7 +13901,7 @@
       <c r="AE32" s="18">
         <v>52.06</v>
       </c>
-      <c r="AF32" s="37">
+      <c r="AF32" s="36">
         <v>0</v>
       </c>
       <c r="AG32" s="37">
@@ -13867,7 +13913,7 @@
       <c r="AI32" s="37">
         <v>0</v>
       </c>
-      <c r="AJ32" s="37">
+      <c r="AJ32" s="62">
         <v>0</v>
       </c>
       <c r="AK32" s="30">
@@ -14010,20 +14056,20 @@
       <c r="AE33" s="19">
         <v>55.57</v>
       </c>
-      <c r="AF33" s="34">
-        <v>26.24</v>
-      </c>
-      <c r="AG33" s="28">
-        <v>72.610000000000099</v>
-      </c>
-      <c r="AH33" s="5">
-        <v>24.05</v>
-      </c>
-      <c r="AI33" s="25">
-        <v>14.54</v>
-      </c>
-      <c r="AJ33" s="22">
-        <v>55.57</v>
+      <c r="AF33" s="41">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="39">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="39">
+        <v>0</v>
+      </c>
+      <c r="AI33" s="39">
+        <v>0</v>
+      </c>
+      <c r="AJ33" s="40">
+        <v>0</v>
       </c>
       <c r="AK33" s="31">
         <v>27.24</v>
@@ -14165,20 +14211,20 @@
       <c r="AE34" s="19">
         <v>59.08</v>
       </c>
-      <c r="AF34" s="34">
-        <v>26.28</v>
-      </c>
-      <c r="AG34" s="28">
-        <v>72.730000000000103</v>
-      </c>
-      <c r="AH34" s="5">
-        <v>24.38</v>
-      </c>
-      <c r="AI34" s="25">
-        <v>17.23</v>
-      </c>
-      <c r="AJ34" s="22">
-        <v>59.08</v>
+      <c r="AF34" s="41">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="39">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="39">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="39">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="40">
+        <v>0</v>
       </c>
       <c r="AK34" s="31">
         <v>27.28</v>
@@ -14320,20 +14366,20 @@
       <c r="AE35" s="19">
         <v>62.59</v>
       </c>
-      <c r="AF35" s="34">
-        <v>26.32</v>
-      </c>
-      <c r="AG35" s="28">
-        <v>72.850000000000193</v>
-      </c>
-      <c r="AH35" s="5">
-        <v>24.71</v>
-      </c>
-      <c r="AI35" s="25">
-        <v>19.920000000000002</v>
-      </c>
-      <c r="AJ35" s="22">
-        <v>62.59</v>
+      <c r="AF35" s="41">
+        <v>0</v>
+      </c>
+      <c r="AG35" s="39">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="39">
+        <v>0</v>
+      </c>
+      <c r="AI35" s="39">
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="40">
+        <v>0</v>
       </c>
       <c r="AK35" s="31">
         <v>27.32</v>
@@ -14475,20 +14521,20 @@
       <c r="AE36" s="20">
         <v>66.099999999999994</v>
       </c>
-      <c r="AF36" s="35">
-        <v>26.36</v>
-      </c>
-      <c r="AG36" s="29">
-        <v>72.970000000000198</v>
-      </c>
-      <c r="AH36" s="6">
-        <v>25.04</v>
-      </c>
-      <c r="AI36" s="26">
-        <v>22.61</v>
-      </c>
-      <c r="AJ36" s="23">
-        <v>66.099999999999994</v>
+      <c r="AF36" s="63">
+        <v>0</v>
+      </c>
+      <c r="AG36" s="64">
+        <v>0</v>
+      </c>
+      <c r="AH36" s="64">
+        <v>0</v>
+      </c>
+      <c r="AI36" s="64">
+        <v>0</v>
+      </c>
+      <c r="AJ36" s="65">
+        <v>0</v>
       </c>
       <c r="AK36" s="32">
         <v>27.36</v>
@@ -14645,19 +14691,19 @@
       <c r="AJ37" s="22">
         <v>69.61</v>
       </c>
-      <c r="AK37" s="41">
-        <v>0</v>
-      </c>
-      <c r="AL37" s="39">
-        <v>0</v>
-      </c>
-      <c r="AM37" s="39">
-        <v>0</v>
-      </c>
-      <c r="AN37" s="39">
-        <v>0</v>
-      </c>
-      <c r="AO37" s="40">
+      <c r="AK37" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL37" s="37">
+        <v>0</v>
+      </c>
+      <c r="AM37" s="37">
+        <v>0</v>
+      </c>
+      <c r="AN37" s="37">
+        <v>0</v>
+      </c>
+      <c r="AO37" s="62">
         <v>0</v>
       </c>
       <c r="AP37" s="34">
@@ -14800,20 +14846,20 @@
       <c r="AJ38" s="22">
         <v>73.12</v>
       </c>
-      <c r="AK38" s="31">
-        <v>27.44</v>
-      </c>
-      <c r="AL38" s="28">
-        <v>73.210000000000207</v>
-      </c>
-      <c r="AM38" s="5">
-        <v>25.7</v>
-      </c>
-      <c r="AN38" s="25">
-        <v>27.99</v>
-      </c>
-      <c r="AO38" s="19">
-        <v>73.12</v>
+      <c r="AK38" s="41">
+        <v>0</v>
+      </c>
+      <c r="AL38" s="39">
+        <v>0</v>
+      </c>
+      <c r="AM38" s="39">
+        <v>0</v>
+      </c>
+      <c r="AN38" s="39">
+        <v>0</v>
+      </c>
+      <c r="AO38" s="40">
+        <v>0</v>
       </c>
       <c r="AP38" s="34">
         <v>28.44</v>
@@ -14955,20 +15001,20 @@
       <c r="AJ39" s="22">
         <v>76.63</v>
       </c>
-      <c r="AK39" s="31">
-        <v>27.48</v>
-      </c>
-      <c r="AL39" s="28">
-        <v>73.330000000000197</v>
-      </c>
-      <c r="AM39" s="5">
-        <v>26.03</v>
-      </c>
-      <c r="AN39" s="25">
-        <v>30.68</v>
-      </c>
-      <c r="AO39" s="19">
-        <v>76.63</v>
+      <c r="AK39" s="41">
+        <v>0</v>
+      </c>
+      <c r="AL39" s="39">
+        <v>0</v>
+      </c>
+      <c r="AM39" s="39">
+        <v>0</v>
+      </c>
+      <c r="AN39" s="39">
+        <v>0</v>
+      </c>
+      <c r="AO39" s="40">
+        <v>0</v>
       </c>
       <c r="AP39" s="34">
         <v>28.48</v>
@@ -15110,20 +15156,20 @@
       <c r="AJ40" s="22">
         <v>80.14</v>
       </c>
-      <c r="AK40" s="31">
-        <v>27.52</v>
-      </c>
-      <c r="AL40" s="28">
-        <v>73.450000000000202</v>
-      </c>
-      <c r="AM40" s="5">
-        <v>26.36</v>
-      </c>
-      <c r="AN40" s="25">
-        <v>33.369999999999997</v>
-      </c>
-      <c r="AO40" s="19">
-        <v>80.14</v>
+      <c r="AK40" s="41">
+        <v>0</v>
+      </c>
+      <c r="AL40" s="39">
+        <v>0</v>
+      </c>
+      <c r="AM40" s="39">
+        <v>0</v>
+      </c>
+      <c r="AN40" s="39">
+        <v>0</v>
+      </c>
+      <c r="AO40" s="40">
+        <v>0</v>
       </c>
       <c r="AP40" s="34">
         <v>28.52</v>
@@ -15265,20 +15311,20 @@
       <c r="AJ41" s="22">
         <v>83.65</v>
       </c>
-      <c r="AK41" s="31">
-        <v>27.56</v>
-      </c>
-      <c r="AL41" s="28">
-        <v>73.570000000000206</v>
-      </c>
-      <c r="AM41" s="5">
-        <v>26.69</v>
-      </c>
-      <c r="AN41" s="25">
-        <v>36.06</v>
-      </c>
-      <c r="AO41" s="19">
-        <v>83.65</v>
+      <c r="AK41" s="63">
+        <v>0</v>
+      </c>
+      <c r="AL41" s="64">
+        <v>0</v>
+      </c>
+      <c r="AM41" s="64">
+        <v>0</v>
+      </c>
+      <c r="AN41" s="64">
+        <v>0</v>
+      </c>
+      <c r="AO41" s="65">
+        <v>0</v>
       </c>
       <c r="AP41" s="34">
         <v>28.56</v>
@@ -15435,7 +15481,7 @@
       <c r="AO42" s="18">
         <v>87.16</v>
       </c>
-      <c r="AP42" s="37">
+      <c r="AP42" s="36">
         <v>0</v>
       </c>
       <c r="AQ42" s="37">
@@ -15447,7 +15493,7 @@
       <c r="AS42" s="37">
         <v>0</v>
       </c>
-      <c r="AT42" s="37">
+      <c r="AT42" s="62">
         <v>0</v>
       </c>
       <c r="AU42" s="30">
@@ -15590,20 +15636,20 @@
       <c r="AO43" s="19">
         <v>90.67</v>
       </c>
-      <c r="AP43" s="34">
-        <v>28.64</v>
-      </c>
-      <c r="AQ43" s="28">
-        <v>73.810000000000201</v>
-      </c>
-      <c r="AR43" s="5">
-        <v>27.35</v>
-      </c>
-      <c r="AS43" s="25">
-        <v>41.44</v>
-      </c>
-      <c r="AT43" s="22">
-        <v>90.67</v>
+      <c r="AP43" s="41">
+        <v>0</v>
+      </c>
+      <c r="AQ43" s="39">
+        <v>0</v>
+      </c>
+      <c r="AR43" s="39">
+        <v>0</v>
+      </c>
+      <c r="AS43" s="39">
+        <v>0</v>
+      </c>
+      <c r="AT43" s="40">
+        <v>0</v>
       </c>
       <c r="AU43" s="31">
         <v>29.64</v>
@@ -15745,20 +15791,20 @@
       <c r="AO44" s="19">
         <v>94.18</v>
       </c>
-      <c r="AP44" s="34">
-        <v>28.68</v>
-      </c>
-      <c r="AQ44" s="28">
-        <v>73.930000000000206</v>
-      </c>
-      <c r="AR44" s="5">
-        <v>27.68</v>
-      </c>
-      <c r="AS44" s="25">
-        <v>44.13</v>
-      </c>
-      <c r="AT44" s="22">
-        <v>94.18</v>
+      <c r="AP44" s="41">
+        <v>0</v>
+      </c>
+      <c r="AQ44" s="39">
+        <v>0</v>
+      </c>
+      <c r="AR44" s="39">
+        <v>0</v>
+      </c>
+      <c r="AS44" s="39">
+        <v>0</v>
+      </c>
+      <c r="AT44" s="40">
+        <v>0</v>
       </c>
       <c r="AU44" s="31">
         <v>29.68</v>
@@ -15900,20 +15946,20 @@
       <c r="AO45" s="19">
         <v>97.69</v>
       </c>
-      <c r="AP45" s="34">
-        <v>28.72</v>
-      </c>
-      <c r="AQ45" s="28">
-        <v>74.050000000000196</v>
-      </c>
-      <c r="AR45" s="5">
-        <v>28.01</v>
-      </c>
-      <c r="AS45" s="25">
-        <v>46.82</v>
-      </c>
-      <c r="AT45" s="22">
-        <v>97.69</v>
+      <c r="AP45" s="41">
+        <v>0</v>
+      </c>
+      <c r="AQ45" s="39">
+        <v>0</v>
+      </c>
+      <c r="AR45" s="39">
+        <v>0</v>
+      </c>
+      <c r="AS45" s="39">
+        <v>0</v>
+      </c>
+      <c r="AT45" s="40">
+        <v>0</v>
       </c>
       <c r="AU45" s="31">
         <v>29.72</v>
@@ -16055,20 +16101,20 @@
       <c r="AO46" s="20">
         <v>1.02</v>
       </c>
-      <c r="AP46" s="35">
-        <v>28.76</v>
-      </c>
-      <c r="AQ46" s="29">
-        <v>74.170000000000201</v>
-      </c>
-      <c r="AR46" s="6">
-        <v>28.34</v>
-      </c>
-      <c r="AS46" s="26">
-        <v>49.51</v>
-      </c>
-      <c r="AT46" s="23">
-        <v>1.02</v>
+      <c r="AP46" s="63">
+        <v>0</v>
+      </c>
+      <c r="AQ46" s="64">
+        <v>0</v>
+      </c>
+      <c r="AR46" s="64">
+        <v>0</v>
+      </c>
+      <c r="AS46" s="64">
+        <v>0</v>
+      </c>
+      <c r="AT46" s="65">
+        <v>0</v>
       </c>
       <c r="AU46" s="32">
         <v>29.76</v>
@@ -16225,19 +16271,19 @@
       <c r="AT47" s="22">
         <v>4.71</v>
       </c>
-      <c r="AU47" s="41">
-        <v>0</v>
-      </c>
-      <c r="AV47" s="39">
-        <v>0</v>
-      </c>
-      <c r="AW47" s="39">
-        <v>0</v>
-      </c>
-      <c r="AX47" s="39">
-        <v>0</v>
-      </c>
-      <c r="AY47" s="40">
+      <c r="AU47" s="36">
+        <v>0</v>
+      </c>
+      <c r="AV47" s="37">
+        <v>0</v>
+      </c>
+      <c r="AW47" s="37">
+        <v>0</v>
+      </c>
+      <c r="AX47" s="37">
+        <v>0</v>
+      </c>
+      <c r="AY47" s="62">
         <v>0</v>
       </c>
     </row>
@@ -16380,20 +16426,20 @@
       <c r="AT48" s="22">
         <v>8.4</v>
       </c>
-      <c r="AU48" s="31">
-        <v>29.84</v>
-      </c>
-      <c r="AV48" s="28">
-        <v>74.410000000000196</v>
-      </c>
-      <c r="AW48" s="5">
-        <v>29</v>
-      </c>
-      <c r="AX48" s="25">
-        <v>54.89</v>
-      </c>
-      <c r="AY48" s="19">
-        <v>8.4</v>
+      <c r="AU48" s="41">
+        <v>0</v>
+      </c>
+      <c r="AV48" s="39">
+        <v>0</v>
+      </c>
+      <c r="AW48" s="39">
+        <v>0</v>
+      </c>
+      <c r="AX48" s="39">
+        <v>0</v>
+      </c>
+      <c r="AY48" s="40">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:51" x14ac:dyDescent="0.25">
@@ -16535,20 +16581,20 @@
       <c r="AT49" s="22">
         <v>12.09</v>
       </c>
-      <c r="AU49" s="31">
-        <v>29.88</v>
-      </c>
-      <c r="AV49" s="28">
-        <v>74.5300000000002</v>
-      </c>
-      <c r="AW49" s="5">
-        <v>29.33</v>
-      </c>
-      <c r="AX49" s="25">
-        <v>57.58</v>
-      </c>
-      <c r="AY49" s="19">
-        <v>12.09</v>
+      <c r="AU49" s="41">
+        <v>0</v>
+      </c>
+      <c r="AV49" s="39">
+        <v>0</v>
+      </c>
+      <c r="AW49" s="39">
+        <v>0</v>
+      </c>
+      <c r="AX49" s="39">
+        <v>0</v>
+      </c>
+      <c r="AY49" s="40">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:51" x14ac:dyDescent="0.25">
@@ -16690,20 +16736,20 @@
       <c r="AT50" s="22">
         <v>15.78</v>
       </c>
-      <c r="AU50" s="31">
-        <v>29.92</v>
-      </c>
-      <c r="AV50" s="28">
-        <v>74.650000000000205</v>
-      </c>
-      <c r="AW50" s="5">
-        <v>29.66</v>
-      </c>
-      <c r="AX50" s="25">
-        <v>60.27</v>
-      </c>
-      <c r="AY50" s="19">
-        <v>15.78</v>
+      <c r="AU50" s="41">
+        <v>0</v>
+      </c>
+      <c r="AV50" s="39">
+        <v>0</v>
+      </c>
+      <c r="AW50" s="39">
+        <v>0</v>
+      </c>
+      <c r="AX50" s="39">
+        <v>0</v>
+      </c>
+      <c r="AY50" s="40">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:51" x14ac:dyDescent="0.25">
@@ -16845,20 +16891,20 @@
       <c r="AT51" s="23">
         <v>19.47</v>
       </c>
-      <c r="AU51" s="32">
-        <v>29.96</v>
-      </c>
-      <c r="AV51" s="29">
-        <v>74.770000000000195</v>
-      </c>
-      <c r="AW51" s="6">
-        <v>29.99</v>
-      </c>
-      <c r="AX51" s="26">
-        <v>62.96</v>
-      </c>
-      <c r="AY51" s="20">
-        <v>19.47</v>
+      <c r="AU51" s="63">
+        <v>0</v>
+      </c>
+      <c r="AV51" s="64">
+        <v>0</v>
+      </c>
+      <c r="AW51" s="64">
+        <v>0</v>
+      </c>
+      <c r="AX51" s="64">
+        <v>0</v>
+      </c>
+      <c r="AY51" s="65">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -16869,10 +16915,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O71"/>
+  <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20:N20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16896,7 +16942,7 @@
       <c r="A3" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="60" t="s">
         <v>66</v>
       </c>
       <c r="M3" s="10"/>
@@ -16905,22 +16951,24 @@
       <c r="A4" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="60"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="C5" s="58"/>
+      <c r="A5" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="60"/>
       <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="58" t="s">
         <v>96</v>
       </c>
       <c r="M6" s="10"/>
@@ -16993,7 +17041,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
-      <c r="B14" s="61"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="17" t="s">
         <v>52</v>
       </c>
@@ -17004,7 +17052,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
-      <c r="B15" s="61"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="17" t="s">
         <v>53</v>
       </c>
@@ -17015,7 +17063,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="44"/>
-      <c r="B16" s="61"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="17" t="s">
         <v>54</v>
       </c>
@@ -17023,7 +17071,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
-      <c r="B17" s="61"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="17" t="s">
         <v>55</v>
       </c>
@@ -17035,23 +17083,23 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="16"/>
-      <c r="C18" s="57"/>
+      <c r="C18" s="56"/>
       <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="16"/>
-      <c r="C19" s="57"/>
+      <c r="C19" s="56"/>
       <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="43"/>
-      <c r="K20" s="56" t="s">
+      <c r="K20" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="61"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="43"/>
@@ -17063,7 +17111,7 @@
       <c r="F21" t="s">
         <v>74</v>
       </c>
-      <c r="O21" s="58" t="s">
+      <c r="O21" s="60" t="s">
         <v>84</v>
       </c>
     </row>
@@ -17083,7 +17131,7 @@
       <c r="K22" t="s">
         <v>63</v>
       </c>
-      <c r="O22" s="58"/>
+      <c r="O22" s="60"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="43"/>
@@ -17091,7 +17139,7 @@
       <c r="C23" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="61"/>
+      <c r="D23" s="59"/>
       <c r="F23" t="s">
         <v>72</v>
       </c>
@@ -17101,7 +17149,7 @@
       <c r="K23" t="s">
         <v>75</v>
       </c>
-      <c r="O23" s="58"/>
+      <c r="O23" s="60"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="43"/>
@@ -17109,8 +17157,8 @@
       <c r="C24" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="61"/>
-      <c r="O24" s="58"/>
+      <c r="D24" s="59"/>
+      <c r="O24" s="60"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="43"/>
@@ -17118,11 +17166,11 @@
       <c r="C25" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="61"/>
+      <c r="D25" s="59"/>
       <c r="F25" t="s">
         <v>76</v>
       </c>
-      <c r="O25" s="58"/>
+      <c r="O25" s="60"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="43"/>
@@ -17135,7 +17183,7 @@
       <c r="K26" t="s">
         <v>63</v>
       </c>
-      <c r="O26" s="58"/>
+      <c r="O26" s="60"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
@@ -17148,11 +17196,11 @@
       <c r="K27" t="s">
         <v>75</v>
       </c>
-      <c r="O27" s="58"/>
+      <c r="O27" s="60"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="43"/>
-      <c r="O28" s="58"/>
+      <c r="O28" s="60"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="43"/>
@@ -17164,7 +17212,7 @@
       <c r="F29" t="s">
         <v>78</v>
       </c>
-      <c r="O29" s="58"/>
+      <c r="O29" s="60"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="43"/>
@@ -17182,7 +17230,7 @@
       <c r="K30" t="s">
         <v>63</v>
       </c>
-      <c r="O30" s="58"/>
+      <c r="O30" s="60"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="43"/>
@@ -17200,20 +17248,20 @@
       <c r="K31" t="s">
         <v>75</v>
       </c>
-      <c r="O31" s="58"/>
+      <c r="O31" s="60"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="43"/>
-      <c r="B32" s="61"/>
+      <c r="B32" s="59"/>
       <c r="C32" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D32" s="9"/>
-      <c r="O32" s="58"/>
+      <c r="O32" s="60"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="43"/>
-      <c r="B33" s="61"/>
+      <c r="B33" s="59"/>
       <c r="C33" s="17" t="s">
         <v>55</v>
       </c>
@@ -17221,9 +17269,9 @@
       <c r="F33" t="s">
         <v>81</v>
       </c>
-      <c r="O33" s="58"/>
+      <c r="O33" s="60"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="43"/>
       <c r="F34" t="s">
         <v>70</v>
@@ -17234,9 +17282,9 @@
       <c r="K34" t="s">
         <v>63</v>
       </c>
-      <c r="O34" s="58"/>
+      <c r="O34" s="60"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="43"/>
       <c r="F35" t="s">
         <v>72</v>
@@ -17247,14 +17295,16 @@
       <c r="K35" t="s">
         <v>75</v>
       </c>
-      <c r="O35" s="58"/>
+      <c r="O35" s="60"/>
     </row>
-    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="43"/>
-      <c r="O36" s="58"/>
+      <c r="O36" s="60"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="43" t="s">
+        <v>99</v>
+      </c>
       <c r="B37" s="49"/>
       <c r="C37" s="17" t="s">
         <v>51</v>
@@ -17263,9 +17313,12 @@
       <c r="F37" t="s">
         <v>83</v>
       </c>
-      <c r="O37" s="58"/>
+      <c r="O37" s="60"/>
+      <c r="P37" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="43"/>
       <c r="B38" s="50"/>
       <c r="C38" s="17" t="s">
@@ -17281,9 +17334,12 @@
       <c r="K38" t="s">
         <v>63</v>
       </c>
-      <c r="O38" s="58"/>
+      <c r="O38" s="60"/>
+      <c r="P38" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="43"/>
       <c r="B39" s="51"/>
       <c r="C39" s="17" t="s">
@@ -17294,35 +17350,44 @@
         <v>72</v>
       </c>
       <c r="G39" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="K39" t="s">
         <v>75</v>
       </c>
-      <c r="O39" s="58"/>
+      <c r="O39" s="60"/>
+      <c r="P39" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="43"/>
       <c r="B40" s="8"/>
       <c r="C40" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D40" s="13"/>
-      <c r="O40" s="58"/>
+      <c r="O40" s="60"/>
+      <c r="P40" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="43"/>
       <c r="B41" s="8"/>
       <c r="C41" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="61"/>
+      <c r="D41" s="59"/>
       <c r="F41" t="s">
         <v>87</v>
       </c>
-      <c r="O41" s="58"/>
+      <c r="O41" s="60"/>
+      <c r="P41" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="43"/>
       <c r="F42" t="s">
         <v>70</v>
@@ -17333,26 +17398,38 @@
       <c r="K42" t="s">
         <v>63</v>
       </c>
-      <c r="O42" s="58"/>
+      <c r="O42" s="60"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="43"/>
       <c r="F43" t="s">
         <v>72</v>
       </c>
       <c r="G43" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="K43" t="s">
         <v>75</v>
       </c>
-      <c r="O43" s="58"/>
+      <c r="O43" s="60"/>
+      <c r="P43" t="s">
+        <v>105</v>
+      </c>
+      <c r="S43" t="s">
+        <v>106</v>
+      </c>
+      <c r="T43" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="43"/>
-      <c r="O44" s="58"/>
+      <c r="O44" s="60"/>
+      <c r="T44" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="43"/>
       <c r="B45" s="49"/>
       <c r="C45" s="17" t="s">
@@ -17362,9 +17439,9 @@
       <c r="F45" t="s">
         <v>88</v>
       </c>
-      <c r="O45" s="58"/>
+      <c r="O45" s="60"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="43"/>
       <c r="B46" s="50"/>
       <c r="C46" s="17" t="s">
@@ -17380,9 +17457,9 @@
       <c r="K46" t="s">
         <v>63</v>
       </c>
-      <c r="O46" s="58"/>
+      <c r="O46" s="60"/>
     </row>
-    <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="43"/>
       <c r="B47" s="51"/>
       <c r="C47" s="17" t="s">
@@ -17398,16 +17475,16 @@
       <c r="K47" t="s">
         <v>75</v>
       </c>
-      <c r="O47" s="58"/>
+      <c r="O47" s="60"/>
     </row>
-    <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="43"/>
       <c r="B48" s="38"/>
       <c r="C48" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D48" s="48"/>
-      <c r="O48" s="58"/>
+      <c r="O48" s="60"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="43"/>
@@ -17419,7 +17496,7 @@
       <c r="F49" t="s">
         <v>91</v>
       </c>
-      <c r="O49" s="58"/>
+      <c r="O49" s="60"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="43"/>
@@ -17432,7 +17509,7 @@
       <c r="K50" t="s">
         <v>63</v>
       </c>
-      <c r="O50" s="58"/>
+      <c r="O50" s="60"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="43"/>
@@ -17445,11 +17522,11 @@
       <c r="K51" t="s">
         <v>75</v>
       </c>
-      <c r="O51" s="58"/>
+      <c r="O51" s="60"/>
     </row>
     <row r="52" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="43"/>
-      <c r="O52" s="58"/>
+      <c r="O52" s="60"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="43"/>
@@ -17461,7 +17538,7 @@
       <c r="F53" t="s">
         <v>92</v>
       </c>
-      <c r="O53" s="58"/>
+      <c r="O53" s="60"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="43"/>
@@ -17479,7 +17556,7 @@
       <c r="K54" t="s">
         <v>75</v>
       </c>
-      <c r="O54" s="58"/>
+      <c r="O54" s="60"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="43"/>
@@ -17497,7 +17574,7 @@
       <c r="K55" t="s">
         <v>75</v>
       </c>
-      <c r="O55" s="58"/>
+      <c r="O55" s="60"/>
     </row>
     <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="43"/>
@@ -17506,7 +17583,7 @@
         <v>54</v>
       </c>
       <c r="D56" s="48"/>
-      <c r="O56" s="58"/>
+      <c r="O56" s="60"/>
     </row>
     <row r="57" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="43"/>
@@ -17515,7 +17592,7 @@
         <v>55</v>
       </c>
       <c r="D57" s="13"/>
-      <c r="O57" s="58"/>
+      <c r="O57" s="60"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="45"/>
@@ -17523,7 +17600,7 @@
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
-      <c r="O58" s="59"/>
+      <c r="O58" s="57"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="16"/>
@@ -17531,7 +17608,7 @@
       <c r="C59" s="16"/>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
-      <c r="O59" s="59"/>
+      <c r="O59" s="57"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="16"/>
@@ -17539,7 +17616,7 @@
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
-      <c r="O60" s="59"/>
+      <c r="O60" s="57"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="16"/>
@@ -17547,7 +17624,7 @@
       <c r="C61" s="16"/>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
-      <c r="O61" s="59"/>
+      <c r="O61" s="57"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="16"/>

</xml_diff>